<commit_message>
:zap: CEC txt to xlsx comparasions +  charts tables
</commit_message>
<xml_diff>
--- a/CEC_txt_to_xlsx/conversions2/RANKTABLE.xlsx
+++ b/CEC_txt_to_xlsx/conversions2/RANKTABLE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="94">
   <si>
     <t>Function No.</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>SOMA</t>
+  </si>
+  <si>
+    <t>VITÓRIAS</t>
   </si>
 </sst>
 </file>
@@ -301,10 +304,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.000_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -323,23 +326,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -361,16 +373,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -386,21 +398,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -415,39 +427,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -466,6 +461,14 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -482,37 +485,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -524,144 +653,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="28">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -871,15 +874,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="0"/>
       </left>
@@ -887,6 +881,19 @@
         <color theme="0"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
@@ -908,19 +915,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -960,6 +954,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -989,180 +1012,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1222,39 +1216,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1605,12 +1599,12 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="A1:G32"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="9.14166666666667" style="1"/>
+    <col min="1" max="1" width="10.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.625" style="2" customWidth="1"/>
     <col min="3" max="3" width="6.375" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.625" style="2" customWidth="1"/>
@@ -2391,30 +2385,41 @@
       <c r="H32" s="30"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="23"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="32"/>
+      <c r="A33" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="24">
+        <v>1</v>
+      </c>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24">
+        <v>17</v>
+      </c>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24">
+        <v>11</v>
+      </c>
+      <c r="G33" s="24"/>
+      <c r="H33" s="27"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="26"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="32"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="31"/>
       <c r="H34" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>